<commit_message>
Adicionado UF à Tabela de Classificação de Estados
</commit_message>
<xml_diff>
--- a/EstadoClassificao.xlsx
+++ b/EstadoClassificao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter\Documents\agilecode\Power BI\Covid-19\Dashboards\Covid-Para\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27545DB4-46B9-45F5-88EB-E3D6150086D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16D5A6D-90A0-4AB8-9B7A-745E1A923859}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E5CAA375-33A5-4239-B8B8-176195C12945}"/>
   </bookViews>
@@ -177,9 +177,6 @@
     <t>Goiás</t>
   </si>
   <si>
-    <t>EstadoFromCSV</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>Goiás (GO)</t>
+  </si>
+  <si>
+    <t>UF</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34C62BB9-0955-4B95-B123-1ACBBFBA86EF}" name="Estado" displayName="Estado" ref="A1:C33" totalsRowShown="0">
   <autoFilter ref="A1:C33" xr:uid="{AECC9709-1446-40A2-8D9E-36DFA4E1DB5B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7D25FEEC-ABAF-4F5E-A0DB-D8ADBB95C2B8}" name="EstadoFromCSV"/>
+    <tableColumn id="1" xr3:uid="{7D25FEEC-ABAF-4F5E-A0DB-D8ADBB95C2B8}" name="UF"/>
     <tableColumn id="2" xr3:uid="{7CDC7D4C-874E-44AC-A35D-C257ADBFA7DF}" name="Estado"/>
     <tableColumn id="5" xr3:uid="{F757EA65-19C8-4D94-8B28-67D377E4E038}" name="Região"/>
   </tableColumns>
@@ -582,9 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27831DEA-8B0A-46E5-A6ED-E6865AA0CFD7}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -594,18 +592,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -649,7 +647,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
@@ -660,7 +658,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
@@ -693,7 +691,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -704,7 +702,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -715,7 +713,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
@@ -737,7 +735,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
@@ -814,7 +812,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
@@ -836,7 +834,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
@@ -858,7 +856,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
@@ -924,7 +922,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>

</xml_diff>